<commit_message>
corrected error in excel file table name for Shop Power Tools, did not rename from base resulting in error
</commit_message>
<xml_diff>
--- a/MAE_Workshop_Inventory_MASTER_TEMPLATE.xlsx
+++ b/MAE_Workshop_Inventory_MASTER_TEMPLATE.xlsx
@@ -1,17 +1,17 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29825"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29725"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/a1a2ae81d67634e6/Desktop/Michanikos Artifex Enterprises/MAE Custom Digital Solutions/Workshop Inventory System and Dashboard/GITHUB_MAE_Workshop Inventory App/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{EF717C5C-A94F-4A9F-962B-1D35F2984CA8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="5" documentId="8_{EF717C5C-A94F-4A9F-962B-1D35F2984CA8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{C495D645-3222-4F78-8BC5-AE4CD207BACD}"/>
   <workbookProtection lockStructure="1"/>
   <bookViews>
-    <workbookView xWindow="5268" yWindow="240" windowWidth="16428" windowHeight="11904" firstSheet="3" activeTab="3" xr2:uid="{BB4209F8-9B83-4E28-9EA3-8709A75F7EFC}"/>
+    <workbookView xWindow="5268" yWindow="240" windowWidth="16428" windowHeight="11904" firstSheet="3" activeTab="4" xr2:uid="{BB4209F8-9B83-4E28-9EA3-8709A75F7EFC}"/>
   </bookViews>
   <sheets>
     <sheet name="Master Dashboard" sheetId="1" r:id="rId1"/>
@@ -214,7 +214,7 @@
     <numFmt numFmtId="164" formatCode="&quot;$&quot;#,##0.00"/>
     <numFmt numFmtId="165" formatCode="mm/dd/yyyy"/>
   </numFmts>
-  <fonts count="1">
+  <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -686,7 +686,7 @@
 </file>
 
 <file path=xl/tables/table5.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="5" xr:uid="{B256D0AD-5808-43AD-9729-C30859C8E0E2}" name="Table5" displayName="Table5" ref="A1:E2" totalsRowShown="0" headerRowDxfId="43" dataDxfId="42">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="5" xr:uid="{B256D0AD-5808-43AD-9729-C30859C8E0E2}" name="Shop_Power_Tools" displayName="Shop_Power_Tools" ref="A1:E2" totalsRowShown="0" headerRowDxfId="43" dataDxfId="42">
   <autoFilter ref="A1:E2" xr:uid="{B256D0AD-5808-43AD-9729-C30859C8E0E2}"/>
   <tableColumns count="5">
     <tableColumn id="1" xr3:uid="{14D3C0F3-786E-4D59-8EBE-4E8ECDF77355}" name="mae_id" dataDxfId="41"/>
@@ -1084,22 +1084,22 @@
   <dimension ref="A1:F1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <pane ySplit="1" topLeftCell="C11" activePane="bottomLeft" state="frozen"/>
+      <pane ySplit="1" topLeftCell="A11" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft" activeCell="C11" sqref="C11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="14.45"/>
+  <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="9" style="1" customWidth="1"/>
     <col min="2" max="2" width="20" style="3" customWidth="1"/>
-    <col min="3" max="3" width="16.42578125" style="2" customWidth="1"/>
-    <col min="4" max="4" width="22.28515625" style="2" customWidth="1"/>
-    <col min="5" max="5" width="22.28515625" style="3" customWidth="1"/>
+    <col min="3" max="3" width="16.44140625" style="2" customWidth="1"/>
+    <col min="4" max="4" width="22.33203125" style="2" customWidth="1"/>
+    <col min="5" max="5" width="22.33203125" style="3" customWidth="1"/>
     <col min="6" max="6" width="21" style="2" customWidth="1"/>
-    <col min="7" max="16384" width="8.85546875" style="6"/>
+    <col min="7" max="16384" width="8.88671875" style="6"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1137,24 +1137,24 @@
       <selection activeCell="C3" sqref="C3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="14.45"/>
+  <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="9" style="1" customWidth="1"/>
-    <col min="2" max="2" width="9.5703125" style="2" customWidth="1"/>
-    <col min="3" max="3" width="31.42578125" style="2" customWidth="1"/>
-    <col min="4" max="4" width="10.5703125" style="2" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="9.5546875" style="2" customWidth="1"/>
+    <col min="3" max="3" width="31.44140625" style="2" customWidth="1"/>
+    <col min="4" max="4" width="10.5546875" style="2" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="17" style="7" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="15.28515625" style="3" customWidth="1"/>
-    <col min="7" max="7" width="16.5703125" style="3" customWidth="1"/>
-    <col min="8" max="8" width="16.7109375" style="5" customWidth="1"/>
-    <col min="9" max="9" width="19.140625" style="2" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="16.7109375" style="3" customWidth="1"/>
-    <col min="11" max="11" width="16.85546875" style="3" customWidth="1"/>
-    <col min="12" max="12" width="22.28515625" style="2" customWidth="1"/>
-    <col min="13" max="16384" width="8.85546875" style="6"/>
+    <col min="6" max="6" width="15.33203125" style="3" customWidth="1"/>
+    <col min="7" max="7" width="16.5546875" style="3" customWidth="1"/>
+    <col min="8" max="8" width="16.6640625" style="5" customWidth="1"/>
+    <col min="9" max="9" width="19.109375" style="2" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="16.6640625" style="3" customWidth="1"/>
+    <col min="11" max="11" width="16.88671875" style="3" customWidth="1"/>
+    <col min="12" max="12" width="22.33203125" style="2" customWidth="1"/>
+    <col min="13" max="16384" width="8.88671875" style="6"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12">
+    <row r="1" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1215,25 +1215,25 @@
   <dimension ref="A1:J1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="J5" sqref="J5"/>
+      <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="14.45"/>
+  <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="9" style="1" customWidth="1"/>
-    <col min="2" max="2" width="9.5703125" style="2" customWidth="1"/>
-    <col min="3" max="3" width="28.7109375" style="2" customWidth="1"/>
-    <col min="4" max="4" width="26.28515625" style="2" customWidth="1"/>
-    <col min="5" max="5" width="14.85546875" style="2" customWidth="1"/>
-    <col min="6" max="6" width="14.7109375" style="7" customWidth="1"/>
-    <col min="7" max="7" width="14.7109375" style="3" customWidth="1"/>
-    <col min="8" max="8" width="12.28515625" style="2" customWidth="1"/>
-    <col min="9" max="9" width="11.42578125" style="6" customWidth="1"/>
-    <col min="10" max="10" width="32.7109375" style="2" customWidth="1"/>
-    <col min="11" max="16384" width="8.85546875" style="6"/>
+    <col min="2" max="2" width="9.5546875" style="2" customWidth="1"/>
+    <col min="3" max="3" width="28.6640625" style="2" customWidth="1"/>
+    <col min="4" max="4" width="26.33203125" style="2" customWidth="1"/>
+    <col min="5" max="5" width="14.88671875" style="2" customWidth="1"/>
+    <col min="6" max="6" width="14.6640625" style="7" customWidth="1"/>
+    <col min="7" max="7" width="14.6640625" style="3" customWidth="1"/>
+    <col min="8" max="8" width="12.33203125" style="2" customWidth="1"/>
+    <col min="9" max="9" width="11.44140625" style="6" customWidth="1"/>
+    <col min="10" max="10" width="32.6640625" style="2" customWidth="1"/>
+    <col min="11" max="16384" width="8.88671875" style="6"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1283,24 +1283,24 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FB7AACC4-9DA2-4A53-AD77-8C5E0C1BF474}">
   <dimension ref="A1:H1"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F7" sqref="F7"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D2" sqref="D2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="14.45"/>
+  <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="9" style="1" customWidth="1"/>
-    <col min="2" max="2" width="7.7109375" style="2" customWidth="1"/>
-    <col min="3" max="3" width="9.5703125" style="2" customWidth="1"/>
-    <col min="4" max="4" width="13.28515625" style="7" customWidth="1"/>
-    <col min="5" max="5" width="13.28515625" style="6" customWidth="1"/>
-    <col min="6" max="6" width="15.85546875" style="6" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="8.7109375" style="3" customWidth="1"/>
-    <col min="8" max="8" width="17.5703125" style="7" customWidth="1"/>
-    <col min="9" max="16384" width="8.85546875" style="6"/>
+    <col min="2" max="2" width="7.6640625" style="2" customWidth="1"/>
+    <col min="3" max="3" width="9.5546875" style="2" customWidth="1"/>
+    <col min="4" max="4" width="13.33203125" style="7" customWidth="1"/>
+    <col min="5" max="5" width="13.33203125" style="6" customWidth="1"/>
+    <col min="6" max="6" width="15.88671875" style="6" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="8.6640625" style="3" customWidth="1"/>
+    <col min="8" max="8" width="17.5546875" style="7" customWidth="1"/>
+    <col min="9" max="16384" width="8.88671875" style="6"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1347,21 +1347,21 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EEDDDAA7-75C3-4AA5-ABFD-D5FB4C627E4C}">
   <dimension ref="A1:E1"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E6" sqref="E6"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C6" sqref="C6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="14.45"/>
+  <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="9" style="1" customWidth="1"/>
-    <col min="2" max="2" width="8.7109375" style="2" customWidth="1"/>
-    <col min="3" max="3" width="72.5703125" style="2" customWidth="1"/>
-    <col min="4" max="4" width="13.140625" style="6" customWidth="1"/>
-    <col min="5" max="5" width="13.5703125" style="6" customWidth="1"/>
-    <col min="6" max="16384" width="8.85546875" style="6"/>
+    <col min="2" max="2" width="8.6640625" style="2" customWidth="1"/>
+    <col min="3" max="3" width="72.5546875" style="2" customWidth="1"/>
+    <col min="4" max="4" width="13.109375" style="6" customWidth="1"/>
+    <col min="5" max="5" width="13.5546875" style="6" customWidth="1"/>
+    <col min="6" max="16384" width="8.88671875" style="6"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1400,20 +1400,20 @@
   <dimension ref="A1:E1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C6" sqref="C6"/>
+      <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="14.45"/>
+  <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="9.28515625" style="1" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="8.7109375" style="2" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="54.7109375" style="2" customWidth="1"/>
-    <col min="4" max="4" width="10.5703125" style="6" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="10.28515625" style="9" bestFit="1" customWidth="1"/>
-    <col min="6" max="16384" width="8.85546875" style="6"/>
+    <col min="1" max="1" width="9.33203125" style="1" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="8.6640625" style="2" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="54.6640625" style="2" customWidth="1"/>
+    <col min="4" max="4" width="10.5546875" style="6" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="10.33203125" style="9" bestFit="1" customWidth="1"/>
+    <col min="6" max="16384" width="8.88671875" style="6"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1452,20 +1452,20 @@
       <selection activeCell="B1" sqref="B1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="14.45"/>
+  <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="9" style="1" customWidth="1"/>
-    <col min="2" max="2" width="41.7109375" style="2" customWidth="1"/>
-    <col min="3" max="3" width="18.42578125" style="2" customWidth="1"/>
-    <col min="4" max="4" width="15.5703125" style="2" customWidth="1"/>
-    <col min="5" max="5" width="14.28515625" style="9" customWidth="1"/>
-    <col min="6" max="6" width="14.140625" style="9" customWidth="1"/>
-    <col min="7" max="7" width="10.42578125" style="3" customWidth="1"/>
-    <col min="8" max="8" width="46.7109375" style="2" customWidth="1"/>
-    <col min="9" max="16384" width="8.85546875" style="6"/>
+    <col min="2" max="2" width="41.6640625" style="2" customWidth="1"/>
+    <col min="3" max="3" width="18.44140625" style="2" customWidth="1"/>
+    <col min="4" max="4" width="15.5546875" style="2" customWidth="1"/>
+    <col min="5" max="5" width="14.33203125" style="9" customWidth="1"/>
+    <col min="6" max="6" width="14.109375" style="9" customWidth="1"/>
+    <col min="7" max="7" width="10.44140625" style="3" customWidth="1"/>
+    <col min="8" max="8" width="46.6640625" style="2" customWidth="1"/>
+    <col min="9" max="16384" width="8.88671875" style="6"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1508,19 +1508,19 @@
       <selection activeCell="D7" sqref="D7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="14.45"/>
+  <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="9" style="1" customWidth="1"/>
-    <col min="2" max="2" width="28.85546875" style="2" customWidth="1"/>
-    <col min="3" max="3" width="60.7109375" style="2" customWidth="1"/>
-    <col min="4" max="4" width="19.28515625" style="2" customWidth="1"/>
-    <col min="5" max="5" width="10.28515625" style="7" customWidth="1"/>
-    <col min="6" max="6" width="9.28515625" style="3" customWidth="1"/>
-    <col min="7" max="7" width="11.28515625" style="2" customWidth="1"/>
-    <col min="8" max="16384" width="8.85546875" style="6"/>
+    <col min="2" max="2" width="28.88671875" style="2" customWidth="1"/>
+    <col min="3" max="3" width="60.6640625" style="2" customWidth="1"/>
+    <col min="4" max="4" width="19.33203125" style="2" customWidth="1"/>
+    <col min="5" max="5" width="10.33203125" style="7" customWidth="1"/>
+    <col min="6" max="6" width="9.33203125" style="3" customWidth="1"/>
+    <col min="7" max="7" width="11.33203125" style="2" customWidth="1"/>
+    <col min="8" max="16384" width="8.88671875" style="6"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1568,21 +1568,21 @@
       <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="14.45"/>
+  <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="9" style="1" customWidth="1"/>
-    <col min="2" max="2" width="30.5703125" style="2" customWidth="1"/>
-    <col min="3" max="3" width="26.28515625" style="2" customWidth="1"/>
+    <col min="2" max="2" width="30.5546875" style="2" customWidth="1"/>
+    <col min="3" max="3" width="26.33203125" style="2" customWidth="1"/>
     <col min="4" max="4" width="17" style="2" customWidth="1"/>
     <col min="5" max="5" width="21" style="2" customWidth="1"/>
-    <col min="6" max="6" width="20.7109375" style="2" customWidth="1"/>
-    <col min="7" max="7" width="12.7109375" style="2" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="15.140625" style="2" customWidth="1"/>
-    <col min="9" max="9" width="32.28515625" style="2" customWidth="1"/>
-    <col min="10" max="16384" width="8.85546875" style="6"/>
+    <col min="6" max="6" width="20.6640625" style="2" customWidth="1"/>
+    <col min="7" max="7" width="12.6640625" style="2" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="15.109375" style="2" customWidth="1"/>
+    <col min="9" max="9" width="32.33203125" style="2" customWidth="1"/>
+    <col min="10" max="16384" width="8.88671875" style="6"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>

</xml_diff>

<commit_message>
updated config.js to add active:true to each column;l rewrote renderTableToUI to hide mae_id (primary key for app to use) from spreadsheet view.
</commit_message>
<xml_diff>
--- a/MAE_Workshop_Inventory_MASTER_TEMPLATE.xlsx
+++ b/MAE_Workshop_Inventory_MASTER_TEMPLATE.xlsx
@@ -8,10 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/a1a2ae81d67634e6/Desktop/Michanikos Artifex Enterprises/MAE Custom Digital Solutions/Workshop Inventory System and Dashboard/GITHUB_MAE_Workshop Inventory App/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="5" documentId="8_{EF717C5C-A94F-4A9F-962B-1D35F2984CA8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{C495D645-3222-4F78-8BC5-AE4CD207BACD}"/>
-  <workbookProtection lockStructure="1"/>
+  <xr:revisionPtr revIDLastSave="7" documentId="8_{EF717C5C-A94F-4A9F-962B-1D35F2984CA8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{D72D3722-99EF-4559-A18B-5ECB6588E0DC}"/>
   <bookViews>
-    <workbookView xWindow="5268" yWindow="240" windowWidth="16428" windowHeight="11904" firstSheet="3" activeTab="4" xr2:uid="{BB4209F8-9B83-4E28-9EA3-8709A75F7EFC}"/>
+    <workbookView xWindow="5268" yWindow="240" windowWidth="16428" windowHeight="11904" firstSheet="6" activeTab="7" xr2:uid="{BB4209F8-9B83-4E28-9EA3-8709A75F7EFC}"/>
   </bookViews>
   <sheets>
     <sheet name="Master Dashboard" sheetId="1" r:id="rId1"/>
@@ -22,7 +21,7 @@
     <sheet name="Shop Hand Tools" sheetId="6" r:id="rId6"/>
     <sheet name="Shop Consumables" sheetId="7" r:id="rId7"/>
     <sheet name="Shop Overhead" sheetId="8" r:id="rId8"/>
-    <sheet name="Supplier Contacts" sheetId="9" r:id="rId9"/>
+    <sheet name="Supplier Contacts" sheetId="9" state="hidden" r:id="rId9"/>
   </sheets>
   <calcPr calcId="191028"/>
   <extLst>
@@ -611,6 +610,10 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
+<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -1347,8 +1350,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EEDDDAA7-75C3-4AA5-ABFD-D5FB4C627E4C}">
   <dimension ref="A1:E1"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C6" sqref="C6"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1504,7 +1507,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3185D484-1AEA-488F-ADB2-C66611F8B5C9}">
   <dimension ref="A1:G1"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="D7" sqref="D7"/>
     </sheetView>
   </sheetViews>

</xml_diff>